<commit_message>
sua lai bai 3
</commit_message>
<xml_diff>
--- a/1A_English/day3.xlsx
+++ b/1A_English/day3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hoc_nodejs\1A_English\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\hoc_nodejs\1A_English\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC192674-5B41-4844-A792-DF7A35BD89AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -151,11 +150,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
@@ -182,8 +189,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -641,11 +649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,10 +743,10 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -767,10 +775,10 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -807,14 +815,15 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>